<commit_message>
alta sucursal con errores
alta sucursal con errores
</commit_message>
<xml_diff>
--- a/ItemsRealizados.xlsx
+++ b/ItemsRealizados.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$4:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$4:$F$54</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>login</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>crear tabla con det login fecha y hs y usuario</t>
+  </si>
+  <si>
+    <t>Quien</t>
   </si>
 </sst>
 </file>
@@ -927,10 +930,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="B3:N1048575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,8 +945,11 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
@@ -958,7 +965,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C5" s="20" t="s">
         <v>2</v>
       </c>
@@ -971,7 +978,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C6" s="21" t="s">
         <v>3</v>
       </c>
@@ -984,7 +991,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C7" s="21" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1004,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="C8" s="21" t="s">
         <v>5</v>
       </c>
@@ -1010,7 +1017,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="21" t="s">
         <v>55</v>
       </c>
@@ -1023,7 +1030,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="3:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
         <v>30</v>
       </c>
@@ -1036,7 +1043,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C11" s="22" t="s">
         <v>6</v>
       </c>
@@ -1049,7 +1056,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C12" s="22" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1069,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C13" s="22" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +1082,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="22" t="s">
         <v>9</v>
       </c>
@@ -1088,7 +1095,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="22" t="s">
         <v>23</v>
       </c>
@@ -1101,7 +1108,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="3:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C16" s="22" t="s">
         <v>25</v>
       </c>
@@ -1114,7 +1121,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C17" s="22" t="s">
         <v>26</v>
       </c>
@@ -1127,7 +1134,7 @@
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C18" s="22" t="s">
         <v>27</v>
       </c>
@@ -1153,7 +1160,7 @@
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C20" s="22" t="s">
         <v>29</v>
       </c>
@@ -1166,7 +1173,7 @@
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="C21" s="21" t="s">
         <v>24</v>
       </c>
@@ -1194,7 +1201,7 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C23" s="21" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1214,7 @@
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C24" s="21" t="s">
         <v>11</v>
       </c>
@@ -1233,7 +1240,7 @@
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C26" s="21" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1253,7 @@
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C27" s="22" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1266,7 @@
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="C28" s="22" t="s">
         <v>51</v>
       </c>
@@ -1272,7 +1279,7 @@
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="C29" s="22" t="s">
         <v>18</v>
       </c>
@@ -1300,7 +1307,7 @@
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="C31" s="22" t="s">
         <v>20</v>
       </c>
@@ -1456,7 +1463,7 @@
       </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="C43" s="22" t="s">
         <v>15</v>
       </c>
@@ -1508,7 +1515,7 @@
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="22" t="s">
         <v>32</v>
@@ -1522,7 +1529,7 @@
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C48" s="21" t="s">
         <v>0</v>
       </c>
@@ -1535,7 +1542,7 @@
       </c>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="C49" s="23" t="s">
         <v>43</v>
       </c>
@@ -1632,7 +1639,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C4:F52"/>
+  <autoFilter ref="C4:F54">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="noecho"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="E5:E54">
     <cfRule type="colorScale" priority="5">
       <colorScale>

</xml_diff>